<commit_message>
Changed the names of chapter 1 ipython notebooks appropriately
</commit_message>
<xml_diff>
--- a/Chapterwise_Ipython_Notebook_Reference.xlsx
+++ b/Chapterwise_Ipython_Notebook_Reference.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="20736" windowHeight="9516"/>
+    <workbookView xWindow="90" yWindow="60" windowWidth="20730" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Content_vs_IPythonNotebook" sheetId="8" r:id="rId1"/>
@@ -313,9 +313,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Step0 - Introduction and Operators.ipynb</t>
-  </si>
-  <si>
     <r>
       <t>o</t>
     </r>
@@ -700,9 +697,6 @@
     </r>
   </si>
   <si>
-    <t>Step0 - Lists.ipynb</t>
-  </si>
-  <si>
     <r>
       <t>§</t>
     </r>
@@ -847,9 +841,6 @@
     </r>
   </si>
   <si>
-    <t>Step0 - Tuples.ipynb</t>
-  </si>
-  <si>
     <r>
       <t>§</t>
     </r>
@@ -970,9 +961,6 @@
     </r>
   </si>
   <si>
-    <t>Step0 - Sets.ipynb</t>
-  </si>
-  <si>
     <r>
       <t>§</t>
     </r>
@@ -1237,9 +1225,6 @@
     </r>
   </si>
   <si>
-    <t>Step0 - Dictionary.ipynb</t>
-  </si>
-  <si>
     <r>
       <t>§</t>
     </r>
@@ -1408,9 +1393,6 @@
     </r>
   </si>
   <si>
-    <t>Step0 - Functions.ipynb</t>
-  </si>
-  <si>
     <r>
       <t>§</t>
     </r>
@@ -1555,9 +1537,6 @@
     </r>
   </si>
   <si>
-    <t>Step0 - File Input and Exception Handling.ipynb</t>
-  </si>
-  <si>
     <r>
       <t>o</t>
     </r>
@@ -2249,6 +2228,27 @@
   </si>
   <si>
     <t>Index: Chapter 5 - Step 5 Text Mining and Recommendation System</t>
+  </si>
+  <si>
+    <t>Introduction and Operators.ipynb</t>
+  </si>
+  <si>
+    <t>Lists.ipynb</t>
+  </si>
+  <si>
+    <t>Tuples.ipynb</t>
+  </si>
+  <si>
+    <t>Sets.ipynb</t>
+  </si>
+  <si>
+    <t>Dictionary.ipynb</t>
+  </si>
+  <si>
+    <t>Functions.ipynb</t>
+  </si>
+  <si>
+    <t>File Input and Exception Handling.ipynb</t>
   </si>
 </sst>
 </file>
@@ -2741,15 +2741,15 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="1.33203125" customWidth="1"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
     <col min="2" max="2" width="65" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
@@ -2762,7 +2762,7 @@
     </row>
     <row r="2" spans="2:4">
       <c r="B2" s="8" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="8"/>
@@ -2852,2194 +2852,2194 @@
         <v>14</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>32</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>39</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>39</v>
+        <v>278</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>39</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>39</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C40" s="26"/>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C43" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C46" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C47" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C48" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C49" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C50" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>45</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C52" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>57</v>
+        <v>280</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C53" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>57</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>57</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="B55" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>57</v>
+        <v>280</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="B56" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>57</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="B57" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C57" s="26"/>
       <c r="D57" s="4"/>
     </row>
     <row r="58" spans="2:4">
       <c r="B58" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C58" s="26"/>
       <c r="D58" s="4"/>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C59" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>65</v>
+        <v>281</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C60" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>65</v>
+        <v>281</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="B61" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C61" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>65</v>
+        <v>281</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="B62" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C62" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>65</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="B63" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C63" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>65</v>
+        <v>281</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C64" s="26"/>
       <c r="D64" s="4"/>
     </row>
     <row r="65" spans="2:4">
       <c r="B65" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C65" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>72</v>
+        <v>282</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="B66" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C66" s="26"/>
       <c r="D66" s="4"/>
     </row>
     <row r="67" spans="2:4">
       <c r="B67" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C67" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>72</v>
+        <v>282</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B69" s="16" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C69" s="27"/>
       <c r="D69" s="16"/>
     </row>
-    <row r="70" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="70" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B70" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C70" s="28"/>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="71" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B71" s="11" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C71" s="29"/>
       <c r="D71" s="12"/>
     </row>
-    <row r="72" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="72" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B72" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C72" s="29"/>
       <c r="D72" s="12"/>
     </row>
-    <row r="73" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="73" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B73" s="14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C73" s="29"/>
       <c r="D73" s="12"/>
     </row>
-    <row r="74" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="74" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B74" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C74" s="29"/>
       <c r="D74" s="12"/>
     </row>
-    <row r="75" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="75" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B75" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C75" s="29"/>
       <c r="D75" s="12"/>
     </row>
-    <row r="76" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="76" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B76" s="13" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C76" s="29"/>
       <c r="D76" s="12"/>
     </row>
-    <row r="77" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="77" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B77" s="13" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C77" s="29"/>
       <c r="D77" s="12"/>
     </row>
-    <row r="78" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="78" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B78" s="14" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C78" s="29"/>
       <c r="D78" s="12"/>
     </row>
-    <row r="79" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="79" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B79" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C79" s="29"/>
       <c r="D79" s="12"/>
     </row>
-    <row r="80" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="80" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B80" s="13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C80" s="29"/>
       <c r="D80" s="12"/>
     </row>
-    <row r="81" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="81" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B81" s="13" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C81" s="29"/>
       <c r="D81" s="12"/>
     </row>
-    <row r="82" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="82" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B82" s="14" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C82" s="29"/>
       <c r="D82" s="12"/>
     </row>
-    <row r="83" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="83" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B83" s="13" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C83" s="29"/>
       <c r="D83" s="12"/>
     </row>
-    <row r="84" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="84" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B84" s="13" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C84" s="29"/>
       <c r="D84" s="12"/>
     </row>
-    <row r="85" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="85" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B85" s="13" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C85" s="29"/>
       <c r="D85" s="12"/>
     </row>
-    <row r="86" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="86" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B86" s="14" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C86" s="29"/>
       <c r="D86" s="12"/>
     </row>
-    <row r="87" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="87" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B87" s="13" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C87" s="29"/>
       <c r="D87" s="12"/>
     </row>
-    <row r="88" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="88" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B88" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C88" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B89" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C89" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B90" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C90" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B91" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C91" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B92" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C92" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B93" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B94" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C88" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D88" s="12" t="s">
+      <c r="C94" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B95" s="13" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="89" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B89" s="14" t="s">
+      <c r="C95" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C89" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D89" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B90" s="14" t="s">
+    </row>
+    <row r="96" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B96" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C90" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B91" s="14" t="s">
+      <c r="C96" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B97" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C91" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B92" s="14" t="s">
+      <c r="C97" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B98" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C92" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D92" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B93" s="14" t="s">
+      <c r="C98" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B99" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C93" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D93" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B94" s="14" t="s">
+      <c r="C99" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B100" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C94" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D94" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B95" s="13" t="s">
+      <c r="C100" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B101" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C95" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D95" s="12" t="s">
+      <c r="C101" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B102" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="96" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B96" s="14" t="s">
+      <c r="C102" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B103" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C96" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D96" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B97" s="14" t="s">
+      <c r="C103" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B104" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C97" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D97" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B98" s="14" t="s">
+      <c r="C104" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B105" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C98" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D98" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B99" s="14" t="s">
+      <c r="C105" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B106" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C99" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D99" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B100" s="14" t="s">
+      <c r="C106" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D106" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C100" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D100" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B101" s="14" t="s">
+    </row>
+    <row r="107" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B107" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C101" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D101" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B102" s="14" t="s">
+      <c r="C107" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B108" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C102" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B103" s="14" t="s">
+      <c r="C108" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B109" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="C103" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D103" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B104" s="14" t="s">
+      <c r="C109" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B110" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C104" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D104" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B105" s="14" t="s">
+      <c r="C110" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B111" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C105" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D105" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B106" s="13" t="s">
+      <c r="C111" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B112" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C106" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D106" s="12" t="s">
+      <c r="C112" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B113" s="14" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="107" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B107" s="14" t="s">
+      <c r="C113" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B114" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C107" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D107" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B108" s="14" t="s">
+      <c r="C114" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B115" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C108" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D108" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B109" s="14" t="s">
+      <c r="C115" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B116" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="C109" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D109" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B110" s="14" t="s">
+      <c r="C116" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B117" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C110" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B111" s="14" t="s">
+      <c r="C117" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B118" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C111" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D111" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B112" s="14" t="s">
+      <c r="C118" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B119" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C112" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D112" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B113" s="14" t="s">
+      <c r="C119" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B120" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C113" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D113" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B114" s="14" t="s">
+      <c r="C120" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B121" s="13" t="s">
         <v>123</v>
-      </c>
-      <c r="C114" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D114" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B115" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C115" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D115" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B116" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C116" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D116" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B117" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C117" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D117" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B118" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C118" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D118" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B119" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C119" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D119" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B120" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C120" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D120" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B121" s="13" t="s">
-        <v>130</v>
       </c>
       <c r="C121" s="29"/>
       <c r="D121" s="12"/>
     </row>
-    <row r="122" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="122" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B122" s="16" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C122" s="27"/>
       <c r="D122" s="16"/>
     </row>
-    <row r="123" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="123" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B123" s="17" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C123" s="28"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="124" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B124" s="18" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C124" s="29"/>
       <c r="D124" s="12"/>
     </row>
-    <row r="125" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="125" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B125" s="11" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C125" s="29"/>
       <c r="D125" s="12"/>
     </row>
-    <row r="126" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="126" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B126" s="18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C126" s="29"/>
       <c r="D126" s="12"/>
     </row>
-    <row r="127" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="127" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B127" s="11" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C127" s="29"/>
       <c r="D127" s="12"/>
     </row>
-    <row r="128" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="128" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B128" s="11" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C128" s="29"/>
       <c r="D128" s="12"/>
     </row>
-    <row r="129" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="129" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B129" s="11" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C129" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="130" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B130" s="11" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C130" s="29"/>
       <c r="D130" s="12"/>
     </row>
-    <row r="131" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="131" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B131" s="19" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C131" s="29"/>
       <c r="D131" s="12"/>
     </row>
-    <row r="132" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="132" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B132" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C132" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B133" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C133" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B134" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C134" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B135" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C135" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D135" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B136" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C136" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D136" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B137" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C132" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D132" s="12" t="s">
+      <c r="C137" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B138" s="11" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="133" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B133" s="11" t="s">
+      <c r="C138" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D138" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B139" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C133" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="134" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B134" s="18" t="s">
+      <c r="C139" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="C134" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D134" s="12" t="s">
+    </row>
+    <row r="140" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B140" s="11" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="135" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B135" s="11" t="s">
+      <c r="C140" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D140" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B141" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="C135" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D135" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="136" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B136" s="11" t="s">
+      <c r="C141" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B142" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C136" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D136" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="137" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B137" s="11" t="s">
+      <c r="C142" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D142" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B143" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="C137" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D137" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="138" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B138" s="11" t="s">
+      <c r="C143" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B144" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C138" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D138" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="139" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B139" s="11" t="s">
+      <c r="C144" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B145" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C139" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D139" s="12" t="s">
+      <c r="C145" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B146" s="11" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="140" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B140" s="11" t="s">
+      <c r="C146" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B147" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C140" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D140" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="141" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B141" s="11" t="s">
+      <c r="C147" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="C141" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D141" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="142" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B142" s="11" t="s">
+    </row>
+    <row r="148" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B148" s="18" t="s">
         <v>156</v>
-      </c>
-      <c r="C142" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D142" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="143" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B143" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C143" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D143" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="144" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B144" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="C144" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D144" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="145" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B145" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C145" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D145" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="146" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B146" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="C146" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D146" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="147" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B147" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C147" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D147" s="12" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B148" s="18" t="s">
-        <v>163</v>
       </c>
       <c r="C148" s="29"/>
       <c r="D148" s="12"/>
     </row>
-    <row r="149" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="149" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B149" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C149" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D149" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B150" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C150" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D150" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B151" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C151" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D151" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B152" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C152" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D152" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B153" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C153" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D153" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B154" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C154" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B155" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C149" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D149" s="12" t="s">
+      <c r="C155" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D155" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="150" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B150" s="11" t="s">
+    <row r="156" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B156" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C150" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D150" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="151" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B151" s="11" t="s">
+      <c r="C156" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156" s="12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B157" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="C151" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D151" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="152" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B152" s="11" t="s">
+      <c r="C157" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D157" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="C152" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D152" s="12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="153" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B153" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="C153" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D153" s="12" t="s">
+    </row>
+    <row r="158" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B158" s="11" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="154" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B154" s="11" t="s">
+      <c r="C158" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D158" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="C154" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D154" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="155" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B155" s="11" t="s">
+    </row>
+    <row r="159" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B159" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C155" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D155" s="12" t="s">
+      <c r="C159" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D159" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="156" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B156" s="11" t="s">
+    <row r="160" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B160" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C156" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D156" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="157" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B157" s="11" t="s">
+      <c r="C160" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D160" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="C157" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D157" s="12" t="s">
+    </row>
+    <row r="161" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B161" s="18" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="158" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B158" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C158" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D158" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B159" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C159" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D159" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B160" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C160" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D160" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="161" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B161" s="18" t="s">
-        <v>182</v>
       </c>
       <c r="C161" s="29"/>
       <c r="D161" s="12"/>
     </row>
-    <row r="162" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="162" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B162" s="11" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C162" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B163" s="11" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C163" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D163" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B164" s="11" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C164" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D164" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B165" s="11" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C165" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D165" s="12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B166" s="18" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C166" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D166" s="12" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="167" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B167" s="16" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C167" s="27"/>
       <c r="D167" s="16"/>
     </row>
-    <row r="168" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="168" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B168" s="17" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C168" s="28"/>
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="169" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B169" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C169" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D169" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B170" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C170" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D170" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B171" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C171" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D171" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B172" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C172" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D172" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B173" s="18" t="s">
         <v>191</v>
-      </c>
-      <c r="C169" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D169" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B170" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="C170" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D170" s="12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B171" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="C171" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D171" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B172" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="C172" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D172" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="173" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B173" s="18" t="s">
-        <v>198</v>
       </c>
       <c r="C173" s="29"/>
       <c r="D173" s="12"/>
     </row>
-    <row r="174" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="174" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B174" s="18" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C174" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D174" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="175" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B175" s="11" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C175" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D175" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B176" s="11" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C176" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D176" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="177" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B177" s="11" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C177" s="29"/>
       <c r="D177" s="12"/>
     </row>
-    <row r="178" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="178" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B178" s="18" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C178" s="29"/>
     </row>
-    <row r="179" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="179" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B179" s="11" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C179" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D179" s="12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="180" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B180" s="11" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C180" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D180" s="12" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="181" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B181" s="11" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C181" s="29"/>
       <c r="D181" s="12"/>
     </row>
-    <row r="182" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="182" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B182" s="11" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C182" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D182" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B183" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C183" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D183" s="12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" s="20" customFormat="1" ht="12">
+      <c r="B184" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C184" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D184" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B185" s="18" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="183" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B183" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="C183" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D183" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4" s="20" customFormat="1" ht="13.8">
-      <c r="B184" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="C184" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D184" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="185" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B185" s="18" t="s">
-        <v>213</v>
       </c>
       <c r="C185" s="29"/>
       <c r="D185" s="12"/>
     </row>
-    <row r="186" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="186" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B186" s="11" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C186" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D186" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="187" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B187" s="11" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C187" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D187" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="188" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B188" s="16" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C188" s="27"/>
       <c r="D188" s="16"/>
     </row>
-    <row r="189" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="189" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B189" s="11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C189" s="28"/>
       <c r="D189" s="10"/>
     </row>
-    <row r="190" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="190" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B190" s="11" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C190" s="29"/>
       <c r="D190" s="12"/>
     </row>
-    <row r="191" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="191" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B191" s="11" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C191" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D191" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="192" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B192" s="11" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C192" s="29"/>
       <c r="D192" s="12"/>
     </row>
-    <row r="193" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="193" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B193" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C193" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B194" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C194" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D194" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B195" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="C195" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D195" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B196" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C196" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D196" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B197" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C197" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D197" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B198" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C198" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B199" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="C193" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D193" s="12" t="s">
+      <c r="C199" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D199" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B200" s="11" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="194" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B194" s="11" t="s">
+      <c r="C200" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D200" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B201" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="C194" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D194" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="195" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B195" s="11" t="s">
+      <c r="C201" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D201" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B202" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C195" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D195" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="196" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B196" s="11" t="s">
+      <c r="C202" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D202" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C196" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D196" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="197" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B197" s="11" t="s">
+    </row>
+    <row r="203" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B203" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="C197" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D197" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="198" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B198" s="11" t="s">
+      <c r="C203" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D203" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B204" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="C198" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D198" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="199" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B199" s="11" t="s">
+      <c r="C204" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D204" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B205" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="C199" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D199" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B200" s="11" t="s">
+      <c r="C205" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D205" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B206" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="C200" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D200" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="201" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B201" s="11" t="s">
+      <c r="C206" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D206" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B207" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="C201" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D201" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="202" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B202" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="C202" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D202" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="203" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B203" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="C203" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D203" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="204" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B204" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C204" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D204" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="205" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B205" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C205" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D205" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="206" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B206" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="C206" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D206" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="207" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B207" s="11" t="s">
-        <v>237</v>
       </c>
       <c r="C207" s="29"/>
       <c r="D207" s="12"/>
     </row>
-    <row r="208" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="208" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B208" s="11" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C208" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D208" s="12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="209" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B209" s="11" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="C209" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D209" s="12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="210" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="210" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B210" s="11" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C210" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D210" s="12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="211" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B211" s="11" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C211" s="29"/>
       <c r="D211" s="12"/>
     </row>
-    <row r="212" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="212" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B212" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C212" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D212" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B213" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C213" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D213" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B214" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C214" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D214" s="12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B215" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C215" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D215" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="216" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B216" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="C212" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D212" s="12" t="s">
+      <c r="C216" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D216" s="12" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="213" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B213" s="11" t="s">
+    <row r="217" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B217" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="C213" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D213" s="12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="214" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B214" s="11" t="s">
+      <c r="C217" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D217" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="C214" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D214" s="12" t="s">
+    </row>
+    <row r="218" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B218" s="11" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="215" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B215" s="11" t="s">
+      <c r="C218" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D218" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="C215" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D215" s="12" t="s">
+    </row>
+    <row r="219" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B219" s="16" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="216" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B216" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="C216" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D216" s="12" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="217" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B217" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="C217" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D217" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="218" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B218" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="C218" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D218" s="12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="219" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B219" s="16" t="s">
-        <v>256</v>
       </c>
       <c r="C219" s="27"/>
       <c r="D219" s="16"/>
     </row>
-    <row r="220" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="220" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B220" s="11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C220" s="28"/>
       <c r="D220" s="10"/>
     </row>
-    <row r="221" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="221" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B221" s="21" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C221" s="29"/>
       <c r="D221" s="12"/>
     </row>
-    <row r="222" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="222" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B222" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="C222" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D222" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B223" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="C223" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D223" s="12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="224" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B224" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C224" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D224" s="12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B225" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="C225" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D225" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="C222" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D222" s="12" t="s">
+    </row>
+    <row r="226" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B226" s="21" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="223" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B223" s="21" t="s">
+      <c r="C226" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D226" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="C223" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D223" s="12" t="s">
+    </row>
+    <row r="227" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B227" s="21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="224" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B224" s="21" t="s">
+      <c r="C227" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D227" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="228" spans="2:4" s="15" customFormat="1" ht="12">
+      <c r="B228" s="21" t="s">
         <v>262</v>
-      </c>
-      <c r="C224" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D224" s="12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="225" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B225" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="C225" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D225" s="12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="226" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B226" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="C226" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D226" s="12" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="227" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B227" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="C227" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D227" s="12" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="228" spans="2:4" s="15" customFormat="1" ht="13.8">
-      <c r="B228" s="21" t="s">
-        <v>269</v>
       </c>
       <c r="C228" s="29"/>
       <c r="D228" s="12"/>
     </row>
-    <row r="229" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="229" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B229" s="11" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C229" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D229" s="12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="230" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="230" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B230" s="11" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C230" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D230" s="12" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="231" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B231" s="21" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C231" s="29"/>
       <c r="D231" s="12"/>
     </row>
-    <row r="232" spans="2:4" s="15" customFormat="1" ht="13.8">
+    <row r="232" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B232" s="11" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C232" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D232" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="233" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B233" s="21" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C233" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D233" s="12" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="234" spans="2:4" s="15" customFormat="1" ht="13.8">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" s="15" customFormat="1" ht="12">
       <c r="B234" s="21" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C234" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D234" s="12" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -5049,29 +5049,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <AlternateThumbnailUrl xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </AlternateThumbnailUrl>
-    <Chapter_x0020_Number xmlns="98582d3f-c513-4300-b6ba-3b60273547d4">1</Chapter_x0020_Number>
-    <ImageCreateDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Description xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Picture" ma:contentTypeID="0x01010200E713CFD383244A45A0CD70FC0E3FA465" ma:contentTypeVersion="" ma:contentTypeDescription="Upload an image or a photograph." ma:contentTypeScope="" ma:versionID="306c00e0b972726df7344d11771934a4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="98582d3f-c513-4300-b6ba-3b60273547d4" xmlns:ns3="9a09a477-a0b4-40c5-9cf7-fb61d98b173f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04c178e20ebc12b73dc15022c485aa46" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5288,26 +5265,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79423943-FE8D-491D-9F77-B97CFAB3ACFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="98582d3f-c513-4300-b6ba-3b60273547d4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE7541D-C0BE-42BD-B498-8587ACF93515}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <AlternateThumbnailUrl xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </AlternateThumbnailUrl>
+    <Chapter_x0020_Number xmlns="98582d3f-c513-4300-b6ba-3b60273547d4">1</Chapter_x0020_Number>
+    <ImageCreateDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Description xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89971926-85B7-4D30-A2B5-F491423BD079}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5325,4 +5306,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE7541D-C0BE-42BD-B498-8587ACF93515}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79423943-FE8D-491D-9F77-B97CFAB3ACFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="98582d3f-c513-4300-b6ba-3b60273547d4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>